<commit_message>
added referencecescesns and rephrase based on professors anotations
</commit_message>
<xml_diff>
--- a/Entregaveis/Relatório de progresso/PlatformComparison.xlsx
+++ b/Entregaveis/Relatório de progresso/PlatformComparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quintela\Desktop\exemplos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quintela\Documents\ISEL\Projecto\ise_learning\Entregaveis\Relatório de progresso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BC8B62-7AEA-4A4A-A3DC-8D18DCDF35EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B2A569-29D8-41A4-8495-A5C5732C67F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30990" yWindow="1650" windowWidth="19800" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>AlgoExpert</t>
   </si>
@@ -126,14 +126,17 @@
     <t>Poor</t>
   </si>
   <si>
-    <t>Enjoyment</t>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>Platform</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +151,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,7 +168,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -165,11 +176,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -177,8 +203,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,57 +504,60 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:20" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>90</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="3">
         <v>7</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K3" s="1"/>
@@ -537,31 +572,31 @@
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="2:20" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="1"/>
@@ -576,31 +611,31 @@
       <c r="T4" s="1"/>
     </row>
     <row r="5" spans="2:20" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <v>14</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K5" s="1"/>
@@ -615,31 +650,31 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="2:20" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K6" s="1"/>
@@ -654,31 +689,31 @@
       <c r="T6" s="1"/>
     </row>
     <row r="7" spans="2:20" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K7" s="1"/>
@@ -693,31 +728,31 @@
       <c r="T7" s="1"/>
     </row>
     <row r="8" spans="2:20" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="3">
         <v>5</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K8" s="1"/>

</xml_diff>